<commit_message>
Changes for EPD curation in Config File
</commit_message>
<xml_diff>
--- a/ConfigFile.xlsx
+++ b/ConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ExploreQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434E0894-5B39-4F20-8B2D-B4010DD59B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388DA96A-8C77-4C90-9E3D-CE67141BC870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="0" windowWidth="19248" windowHeight="11772" xr2:uid="{7D5AD391-3090-4A17-A83F-77933628267E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7D5AD391-3090-4A17-A83F-77933628267E}"/>
   </bookViews>
   <sheets>
     <sheet name="ConfigurationSheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="196">
   <si>
     <t>Parameter Extraction Module</t>
   </si>
@@ -621,6 +621,12 @@
   </si>
   <si>
     <t>/data/RAD/share/EPAD/EPAD500.0/analysis/Population/MotionASL</t>
+  </si>
+  <si>
+    <t>SSE_im</t>
+  </si>
+  <si>
+    <t>DTIfit_sse.nii</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -695,6 +701,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1011,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DB9FB8-9BC8-41E3-B64B-BC7675F5CE89}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1036,7 @@
     <col min="7" max="7" width="40.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1040,30 +1049,28 @@
       <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
+      <c r="G1" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="G2" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
@@ -1071,249 +1078,274 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="9" t="s">
-        <v>182</v>
-      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="G7" s="7" t="s">
-        <v>183</v>
-      </c>
+    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="10"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>190</v>
-      </c>
+      <c r="G8" s="10"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>191</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>175</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>176</v>
-      </c>
+      <c r="G12" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>151</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1479,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992C5751-B2FF-495D-A24F-B5C98DCFD044}">
   <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Configuration file for vIMI
</commit_message>
<xml_diff>
--- a/ConfigFile.xlsx
+++ b/ConfigFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ExploreQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\Home\Github\ExploreQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14893FD-D742-433F-B9FC-4004E2762940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFED6EB-E6F4-4398-A894-D80E84BA8EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33315" yWindow="510" windowWidth="21600" windowHeight="11325" xr2:uid="{7D5AD391-3090-4A17-A83F-77933628267E}"/>
+    <workbookView xWindow="642" yWindow="492" windowWidth="21600" windowHeight="11010" xr2:uid="{7D5AD391-3090-4A17-A83F-77933628267E}"/>
   </bookViews>
   <sheets>
     <sheet name="ConfigurationSheet" sheetId="1" r:id="rId1"/>
@@ -611,9 +611,6 @@
     <t>DTIfit_sse.nii</t>
   </si>
   <si>
-    <t>\d{3}EPAD\d{5}_1</t>
-  </si>
-  <si>
     <t>SD.nii</t>
   </si>
   <si>
@@ -623,16 +620,19 @@
     <t>D:\Lavoro\EPAD_tobecopied</t>
   </si>
   <si>
-    <t>/radshare/EPAD/EPAD_rerun/analysis/Population/MotionASL</t>
-  </si>
-  <si>
-    <t>/radshare/EPAD/EPAD1500.0_eligible</t>
-  </si>
-  <si>
     <t>/radshare/EPAD/scripts/ExploreASL</t>
   </si>
   <si>
     <t>T1_ORI.nii</t>
+  </si>
+  <si>
+    <t>/radshare/EPAD/EPAD_repository/analysis</t>
+  </si>
+  <si>
+    <t>\d{3}EPAD\d{5}_\d</t>
+  </si>
+  <si>
+    <t>/radshare/EPAD/EPAD_repository/analysis/Population/MotionASL</t>
   </si>
 </sst>
 </file>
@@ -1028,21 +1028,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DB9FB8-9BC8-41E3-B64B-BC7675F5CE89}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="40.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.3125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="37.41796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.89453125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5234375" customWidth="1"/>
+    <col min="7" max="7" width="40.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="5"/>
@@ -1068,7 +1068,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1130,19 +1130,19 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" s="10"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="G8" s="10"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1153,32 +1153,32 @@
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>173</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>174</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>175</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>176</v>
       </c>
@@ -1237,12 +1237,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>159</v>
@@ -1251,7 +1251,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>160</v>
       </c>
@@ -1262,15 +1262,15 @@
         <v>160</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>161</v>
@@ -1279,7 +1279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>169</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
         <v>152</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
         <v>151</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>153</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>163</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>165</v>
       </c>
@@ -1330,15 +1330,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
         <v>170</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>188</v>
       </c>
@@ -1368,15 +1368,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.5234375" customWidth="1"/>
+    <col min="2" max="2" width="13.3125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>139</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>147</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>186</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -1521,16 +1521,16 @@
       <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" customWidth="1"/>
-    <col min="4" max="4" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.20703125" customWidth="1"/>
+    <col min="3" max="3" width="29.41796875" customWidth="1"/>
+    <col min="4" max="4" width="43.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>132</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>3</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>3</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>3</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>3</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>3</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>3</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -3728,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>3</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>3</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>3</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>3</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>3</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>3</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>3</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>3</v>
       </c>

</xml_diff>